<commit_message>
Fixing the unit test documentation
</commit_message>
<xml_diff>
--- a/Documents/Blog Application Unit Test Scenarios.xlsx
+++ b/Documents/Blog Application Unit Test Scenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="88">
   <si>
     <t>Unit Test Scenarios</t>
   </si>
@@ -1005,12 +1005,6 @@
   </si>
   <si>
     <t xml:space="preserve">Users edit their comments </t>
-  </si>
-  <si>
-    <t>Click Account Information in Client Store Form.</t>
-  </si>
-  <si>
-    <t>Account Form should appear</t>
   </si>
   <si>
     <t>Type in valid password in password  textbox.
@@ -1177,6 +1171,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1184,14 +1185,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1199,13 +1201,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1219,16 +1214,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1242,26 +1246,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1282,31 +1270,37 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1350,7 +1344,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1362,139 +1482,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1512,19 +1512,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1570,24 +1564,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1603,6 +1593,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1631,178 +1630,173 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2186,10 +2180,10 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2197,10 +2191,10 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2208,10 +2202,10 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2233,7 +2227,7 @@
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2252,10 +2246,10 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2263,10 +2257,10 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2274,10 +2268,10 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2285,10 +2279,10 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2326,10 +2320,10 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2337,10 +2331,10 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2362,7 +2356,7 @@
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2381,10 +2375,10 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2392,10 +2386,10 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2403,10 +2397,10 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2414,10 +2408,10 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2425,10 +2419,10 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3024,10 +3018,10 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3035,10 +3029,10 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3049,7 +3043,7 @@
       <c r="B4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3057,10 +3051,10 @@
       <c r="A5" s="1">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3068,10 +3062,10 @@
       <c r="A6" s="1">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3079,10 +3073,10 @@
       <c r="A7" s="1">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3090,10 +3084,10 @@
       <c r="A8" s="1">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3101,10 +3095,10 @@
       <c r="A9" s="1">
         <v>10</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3117,10 +3111,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -3138,9 +3132,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" ht="60" spans="1:3">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>75</v>
@@ -3151,134 +3145,123 @@
     </row>
     <row r="3" ht="60" spans="1:3">
       <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" ht="60" spans="1:3">
       <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>80</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" ht="60" spans="1:3">
       <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" ht="60" spans="1:3">
       <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" ht="60" spans="1:3">
       <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" ht="60" spans="1:3">
       <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" ht="60" spans="1:3">
       <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" ht="75" spans="1:3">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" ht="60" spans="1:3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" ht="75" spans="1:3">
       <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" ht="75" spans="1:3">
       <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>88</v>
+      <c r="C12" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" ht="75" spans="1:3">
       <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" ht="75" spans="1:3">
-      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>88</v>
+      <c r="B13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>